<commit_message>
writing data rows (Tue May  9 18:34:54 2023)
</commit_message>
<xml_diff>
--- a/dict_test.xlsx
+++ b/dict_test.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="25">
   <si>
     <t>Population Changes</t>
   </si>
@@ -24,20 +24,80 @@
     <t>Metric</t>
   </si>
   <si>
+    <t>Scenario 1</t>
+  </si>
+  <si>
+    <t>Scenario 2</t>
+  </si>
+  <si>
+    <t>Scenario 3</t>
+  </si>
+  <si>
+    <t>Scenario 4</t>
+  </si>
+  <si>
+    <t>Scenario 5</t>
+  </si>
+  <si>
     <t>Compare loaded scenarios...</t>
   </si>
   <si>
+    <t>FER</t>
+  </si>
+  <si>
+    <t>Demo 2</t>
+  </si>
+  <si>
+    <t>Demo 1</t>
+  </si>
+  <si>
+    <t>FEW</t>
+  </si>
+  <si>
     <t>Infrastructure Changes</t>
   </si>
   <si>
+    <t>Lane Length by FER</t>
+  </si>
+  <si>
+    <t>Something by FER</t>
+  </si>
+  <si>
+    <t>Lane Length by FEW</t>
+  </si>
+  <si>
+    <t>Something by FEW</t>
+  </si>
+  <si>
+    <t>FEL</t>
+  </si>
+  <si>
+    <t>Train service kms</t>
+  </si>
+  <si>
     <t>Rituals</t>
+  </si>
+  <si>
+    <t>Trains</t>
+  </si>
+  <si>
+    <t>Buses</t>
+  </si>
+  <si>
+    <t>Trams</t>
+  </si>
+  <si>
+    <t>Horse and Carriage</t>
+  </si>
+  <si>
+    <t>Hose and Carriage</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -53,6 +113,12 @@
     </font>
     <font>
       <b/>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Segoe UI (Body)"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="8"/>
       <color theme="1"/>
       <name val="Segoe UI (Body)"/>
@@ -79,7 +145,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -87,17 +153,89 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF9B9B9B"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF9B9B9B"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF9B9B9B"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF9B9B9B"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF9B9B9B"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF9B9B9B"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF9B9B9B"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF9B9B9B"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF9B9B9B"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF9B9B9B"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF9B9B9B"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF9B9B9B"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF9B9B9B"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF9B9B9B"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -393,31 +531,139 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="44" customWidth="1"/>
+    <col min="1" max="1" width="35.5703125" customWidth="1"/>
     <col min="6" max="6" width="3" customWidth="1"/>
     <col min="7" max="7" width="0" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18" customHeight="1">
+    <row r="1" spans="1:12" ht="18" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="18" customHeight="1">
+    <row r="2" spans="1:12" ht="18" customHeight="1">
       <c r="A2" s="1"/>
       <c r="B2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="36" customHeight="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="36" customHeight="1">
       <c r="A3" s="2" t="s">
         <v>1</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="L3" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="H6">
+        <v>6464470.35</v>
+      </c>
+      <c r="I6">
+        <v>8862726.237</v>
+      </c>
+      <c r="J6">
+        <v>9062726.237</v>
+      </c>
+      <c r="K6">
+        <v>9262726.237</v>
+      </c>
+      <c r="L6">
+        <v>9462726.237</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="H7">
+        <v>3218647.34</v>
+      </c>
+      <c r="I7">
+        <v>4553387.284</v>
+      </c>
+      <c r="J7">
+        <v>4753387.284</v>
+      </c>
+      <c r="K7">
+        <v>4953387.284</v>
+      </c>
+      <c r="L7">
+        <v>5153387.284</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="H9">
+        <v>2512728.79</v>
+      </c>
+      <c r="I9">
+        <v>3485670.148</v>
+      </c>
+      <c r="J9">
+        <v>3685670.148</v>
+      </c>
+      <c r="K9">
+        <v>3885670.148</v>
+      </c>
+      <c r="L9">
+        <v>4085670.148</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="H12">
+        <v>1628963.25</v>
+      </c>
+      <c r="I12">
+        <v>2367808.709</v>
+      </c>
+      <c r="J12">
+        <v>2567808.709</v>
+      </c>
+      <c r="K12">
+        <v>2767808.709</v>
+      </c>
+      <c r="L12">
+        <v>2967808.709</v>
       </c>
     </row>
   </sheetData>
@@ -431,31 +677,307 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:L24"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="44" customWidth="1"/>
+    <col min="1" max="1" width="35.5703125" customWidth="1"/>
     <col min="6" max="6" width="3" customWidth="1"/>
     <col min="7" max="7" width="0" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18" customHeight="1">
+    <row r="1" spans="1:12" ht="18" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="18" customHeight="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="18" customHeight="1">
       <c r="A2" s="1"/>
       <c r="B2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="36" customHeight="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="36" customHeight="1">
       <c r="A3" s="2" t="s">
         <v>1</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="L3" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="H6">
+        <v>6464470.35</v>
+      </c>
+      <c r="I6">
+        <v>8862726.237</v>
+      </c>
+      <c r="J6">
+        <v>9062726.237</v>
+      </c>
+      <c r="K6">
+        <v>9262726.237</v>
+      </c>
+      <c r="L6">
+        <v>9462726.237</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="H7">
+        <v>3218647.34</v>
+      </c>
+      <c r="I7">
+        <v>4553387.284</v>
+      </c>
+      <c r="J7">
+        <v>4753387.284</v>
+      </c>
+      <c r="K7">
+        <v>4953387.284</v>
+      </c>
+      <c r="L7">
+        <v>5153387.284</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="H8">
+        <v>2512728.79</v>
+      </c>
+      <c r="I8">
+        <v>3485670.148</v>
+      </c>
+      <c r="J8">
+        <v>3685670.148</v>
+      </c>
+      <c r="K8">
+        <v>3885670.148</v>
+      </c>
+      <c r="L8">
+        <v>4085670.148</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="H10">
+        <v>1628963.25</v>
+      </c>
+      <c r="I10">
+        <v>2367808.709</v>
+      </c>
+      <c r="J10">
+        <v>2567808.709</v>
+      </c>
+      <c r="K10">
+        <v>2767808.709</v>
+      </c>
+      <c r="L10">
+        <v>2967808.709</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="H11">
+        <v>6464470.35</v>
+      </c>
+      <c r="I11">
+        <v>8862726.237</v>
+      </c>
+      <c r="J11">
+        <v>9062726.237</v>
+      </c>
+      <c r="K11">
+        <v>9262726.237</v>
+      </c>
+      <c r="L11">
+        <v>9462726.237</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="H12">
+        <v>3218647.34</v>
+      </c>
+      <c r="I12">
+        <v>4553387.284</v>
+      </c>
+      <c r="J12">
+        <v>4753387.284</v>
+      </c>
+      <c r="K12">
+        <v>4953387.284</v>
+      </c>
+      <c r="L12">
+        <v>5153387.284</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="A14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="H15">
+        <v>6464470.35</v>
+      </c>
+      <c r="I15">
+        <v>8862726.237</v>
+      </c>
+      <c r="J15">
+        <v>9062726.237</v>
+      </c>
+      <c r="K15">
+        <v>9262726.237</v>
+      </c>
+      <c r="L15">
+        <v>9462726.237</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="H16">
+        <v>3218647.34</v>
+      </c>
+      <c r="I16">
+        <v>4553387.284</v>
+      </c>
+      <c r="J16">
+        <v>4753387.284</v>
+      </c>
+      <c r="K16">
+        <v>4953387.284</v>
+      </c>
+      <c r="L16">
+        <v>5153387.284</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12">
+      <c r="H17">
+        <v>2512728.79</v>
+      </c>
+      <c r="I17">
+        <v>3485670.148</v>
+      </c>
+      <c r="J17">
+        <v>3685670.148</v>
+      </c>
+      <c r="K17">
+        <v>3885670.148</v>
+      </c>
+      <c r="L17">
+        <v>4085670.148</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12">
+      <c r="A18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12">
+      <c r="H19">
+        <v>1628963.25</v>
+      </c>
+      <c r="I19">
+        <v>2367808.709</v>
+      </c>
+      <c r="J19">
+        <v>2567808.709</v>
+      </c>
+      <c r="K19">
+        <v>2767808.709</v>
+      </c>
+      <c r="L19">
+        <v>2967808.709</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12">
+      <c r="H20">
+        <v>6464470.35</v>
+      </c>
+      <c r="I20">
+        <v>8862726.237</v>
+      </c>
+      <c r="J20">
+        <v>9062726.237</v>
+      </c>
+      <c r="K20">
+        <v>9262726.237</v>
+      </c>
+      <c r="L20">
+        <v>9462726.237</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12">
+      <c r="H21">
+        <v>3218647.34</v>
+      </c>
+      <c r="I21">
+        <v>4553387.284</v>
+      </c>
+      <c r="J21">
+        <v>4753387.284</v>
+      </c>
+      <c r="K21">
+        <v>4953387.284</v>
+      </c>
+      <c r="L21">
+        <v>5153387.284</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12">
+      <c r="A22" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12">
+      <c r="A23" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12">
+      <c r="H24">
+        <v>2512728.79</v>
+      </c>
+      <c r="I24">
+        <v>3485670.148</v>
+      </c>
+      <c r="J24">
+        <v>3685670.148</v>
+      </c>
+      <c r="K24">
+        <v>3885670.148</v>
+      </c>
+      <c r="L24">
+        <v>4085670.148</v>
       </c>
     </row>
   </sheetData>
@@ -469,31 +991,205 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="44" customWidth="1"/>
+    <col min="1" max="1" width="35.5703125" customWidth="1"/>
     <col min="6" max="6" width="3" customWidth="1"/>
     <col min="7" max="7" width="0" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18" customHeight="1">
+    <row r="1" spans="1:12" ht="18" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="18" customHeight="1">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="18" customHeight="1">
       <c r="A2" s="1"/>
       <c r="B2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="36" customHeight="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="36" customHeight="1">
       <c r="A3" s="2" t="s">
         <v>1</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="L3" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="H6">
+        <v>1628963.25</v>
+      </c>
+      <c r="I6">
+        <v>2367808.709</v>
+      </c>
+      <c r="J6">
+        <v>2567808.709</v>
+      </c>
+      <c r="K6">
+        <v>2767808.709</v>
+      </c>
+      <c r="L6">
+        <v>2967808.709</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="H7">
+        <v>2512728.79</v>
+      </c>
+      <c r="I7">
+        <v>3485670.148</v>
+      </c>
+      <c r="J7">
+        <v>3685670.148</v>
+      </c>
+      <c r="K7">
+        <v>3885670.148</v>
+      </c>
+      <c r="L7">
+        <v>4085670.148</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="A8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="H9">
+        <v>1628963.25</v>
+      </c>
+      <c r="I9">
+        <v>2367808.709</v>
+      </c>
+      <c r="J9">
+        <v>2567808.709</v>
+      </c>
+      <c r="K9">
+        <v>2767808.709</v>
+      </c>
+      <c r="L9">
+        <v>2967808.709</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="A11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="H12">
+        <v>6464470.35</v>
+      </c>
+      <c r="I12">
+        <v>8862726.237</v>
+      </c>
+      <c r="J12">
+        <v>9062726.237</v>
+      </c>
+      <c r="K12">
+        <v>9262726.237</v>
+      </c>
+      <c r="L12">
+        <v>9462726.237</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="A13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="H14">
+        <v>3218647.34</v>
+      </c>
+      <c r="I14">
+        <v>4553387.284</v>
+      </c>
+      <c r="J14">
+        <v>4753387.284</v>
+      </c>
+      <c r="K14">
+        <v>4953387.284</v>
+      </c>
+      <c r="L14">
+        <v>5153387.284</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="A15" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="H16">
+        <v>2512728.79</v>
+      </c>
+      <c r="I16">
+        <v>3485670.148</v>
+      </c>
+      <c r="J16">
+        <v>3685670.148</v>
+      </c>
+      <c r="K16">
+        <v>3885670.148</v>
+      </c>
+      <c r="L16">
+        <v>4085670.148</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12">
+      <c r="A17" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12">
+      <c r="H18">
+        <v>1628963.25</v>
+      </c>
+      <c r="I18">
+        <v>2367808.709</v>
+      </c>
+      <c r="J18">
+        <v>2567808.709</v>
+      </c>
+      <c r="K18">
+        <v>2767808.709</v>
+      </c>
+      <c r="L18">
+        <v>2967808.709</v>
       </c>
     </row>
   </sheetData>

</xml_diff>